<commit_message>
Pushing after successful calibration progress in v12 with limited param set and beginning to explore the full param set in v13 with limited sample volume (to aid in GPR and cut steps)
</commit_message>
<xml_diff>
--- a/v12_restricted_params/Params.xlsx
+++ b/v12_restricted_params/Params.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\Malaria-Uganda-PRISM\v12_restricted_params\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E767ABC-1DDB-45AD-83BD-9BD82BDC81F4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C717057D-8B3B-4EB1-9486-0B8D3A045A7F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2033" yWindow="2460" windowWidth="16874" windowHeight="10523" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>